<commit_message>
updates name of zoop data to be consistant with others
</commit_message>
<xml_diff>
--- a/data-raw/metadata/F4F2021_metadata.xlsx
+++ b/data-raw/metadata/F4F2021_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erin Cain\Documents\Git\CVPIA\data-stewardship\EDI_data_repos_to_upload\fish-food-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF36301-5A70-46DE-BC3D-BF1349A9047E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A3E23A-3FE3-47E4-8A47-E590C9AF66F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="-12540" windowWidth="16350" windowHeight="7875" tabRatio="543" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="543" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="personnel" sheetId="1" r:id="rId1"/>
@@ -1522,7 +1522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1925,8 +1925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1970,13 +1970,13 @@
         <v>-121.79667600000001</v>
       </c>
       <c r="C2" s="2">
-        <v>-121.78950500000001</v>
+        <v>-121.723641</v>
       </c>
       <c r="D2" s="2">
         <v>38.867317999999997</v>
       </c>
       <c r="E2" s="2">
-        <v>38.861376999999997</v>
+        <v>38.851730000000003</v>
       </c>
       <c r="F2" s="10">
         <v>43417</v>

</xml_diff>